<commit_message>
one more minor update
</commit_message>
<xml_diff>
--- a/bugs analyses/Assessment_Benchmarks/Parameter_Impaired.xlsx
+++ b/bugs analyses/Assessment_Benchmarks/Parameter_Impaired.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateoforegon-my.sharepoint.com/personal/lesley_merrick_deq_oregon_gov/Documents/Microsoft Teams Data/New folder/BioMonORDEQ/bugs analyses/Assessment_Benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{92768450-F0F4-4B03-AF7F-2595CAB33A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8AD9CFB-96F3-466C-A7FB-BFA707E57085}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{92768450-F0F4-4B03-AF7F-2595CAB33A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BF1D4A0-3AEF-4D0D-B891-C0F504D81EE3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4FADE6FC-D746-4C41-A819-63DD57A7812C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{4FADE6FC-D746-4C41-A819-63DD57A7812C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SR" sheetId="1" r:id="rId1"/>
+    <sheet name="WS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AF$382</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$AA$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SR!$A$1:$AF$382</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">WS!$A$1:$AA$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5732,7 +5732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A7535B-B041-4A9F-B0A9-A6D2B476997E}">
   <dimension ref="A1:AE382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -10966,7 +10966,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>245</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>255</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>255</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>255</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>269</v>
       </c>
@@ -11916,7 +11916,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>285</v>
       </c>
@@ -12296,7 +12296,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>307</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>316</v>
       </c>
@@ -12961,7 +12961,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>330</v>
       </c>
@@ -13436,7 +13436,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>342</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>355</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>364</v>
       </c>
@@ -14386,7 +14386,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>374</v>
       </c>
@@ -15146,7 +15146,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>410</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>423</v>
       </c>
@@ -15716,7 +15716,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>423</v>
       </c>
@@ -15811,7 +15811,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>440</v>
       </c>
@@ -16191,7 +16191,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>451</v>
       </c>
@@ -16381,7 +16381,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="113" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>451</v>
       </c>
@@ -16476,7 +16476,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="114" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>461</v>
       </c>
@@ -16666,7 +16666,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>466</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="120" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:31" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>466</v>
       </c>
@@ -17141,7 +17141,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="121" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>483</v>
       </c>
@@ -17331,7 +17331,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="123" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>483</v>
       </c>
@@ -17901,7 +17901,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="129" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>501</v>
       </c>
@@ -17996,7 +17996,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="130" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>501</v>
       </c>
@@ -18471,7 +18471,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="135" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>517</v>
       </c>
@@ -18566,7 +18566,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="136" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:31" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>517</v>
       </c>
@@ -18756,7 +18756,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="138" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>528</v>
       </c>
@@ -19041,7 +19041,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="141" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>532</v>
       </c>
@@ -20086,7 +20086,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="152" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>587</v>
       </c>
@@ -20466,7 +20466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="156" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>600</v>
       </c>
@@ -20751,7 +20751,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="159" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>600</v>
       </c>
@@ -20846,7 +20846,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="160" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>600</v>
       </c>
@@ -21226,7 +21226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>623</v>
       </c>
@@ -21416,7 +21416,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="166" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>633</v>
       </c>
@@ -21511,7 +21511,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="167" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>640</v>
       </c>
@@ -21606,7 +21606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="168" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>640</v>
       </c>
@@ -22271,7 +22271,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="175" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>679</v>
       </c>
@@ -22366,7 +22366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="176" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>685</v>
       </c>
@@ -23791,7 +23791,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="191" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>731</v>
       </c>
@@ -23981,7 +23981,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>741</v>
       </c>
@@ -24361,7 +24361,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>748</v>
       </c>
@@ -24741,7 +24741,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="201" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>772</v>
       </c>
@@ -24836,7 +24836,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="202" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>772</v>
       </c>
@@ -24931,7 +24931,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="203" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>781</v>
       </c>
@@ -25026,7 +25026,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="204" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>781</v>
       </c>
@@ -25216,7 +25216,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="206" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:31" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>792</v>
       </c>
@@ -25406,7 +25406,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="208" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>804</v>
       </c>
@@ -25501,7 +25501,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="209" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>804</v>
       </c>
@@ -25596,7 +25596,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="210" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>804</v>
       </c>
@@ -26071,7 +26071,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="215" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>834</v>
       </c>
@@ -26356,7 +26356,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="218" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>848</v>
       </c>
@@ -27021,7 +27021,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="225" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>861</v>
       </c>
@@ -27116,7 +27116,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="226" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>884</v>
       </c>
@@ -27211,7 +27211,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="227" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>884</v>
       </c>
@@ -27306,7 +27306,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="228" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>891</v>
       </c>
@@ -27401,7 +27401,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="229" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>896</v>
       </c>
@@ -28066,7 +28066,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="236" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>915</v>
       </c>
@@ -28161,7 +28161,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="237" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>920</v>
       </c>
@@ -29016,7 +29016,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="246" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>955</v>
       </c>
@@ -29491,7 +29491,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="251" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>974</v>
       </c>
@@ -29586,7 +29586,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="252" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>979</v>
       </c>
@@ -29776,7 +29776,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="254" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>985</v>
       </c>
@@ -29871,7 +29871,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="255" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>985</v>
       </c>
@@ -29966,7 +29966,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="256" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>985</v>
       </c>
@@ -30156,7 +30156,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="258" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>985</v>
       </c>
@@ -30251,7 +30251,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="259" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>998</v>
       </c>
@@ -30346,7 +30346,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="260" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>1004</v>
       </c>
@@ -30536,7 +30536,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="262" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>1012</v>
       </c>
@@ -30821,7 +30821,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="265" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>1020</v>
       </c>
@@ -31581,7 +31581,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="273" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>1048</v>
       </c>
@@ -31961,7 +31961,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="277" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>1055</v>
       </c>
@@ -33196,7 +33196,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="290" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>1091</v>
       </c>
@@ -33291,7 +33291,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="291" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:31" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>1091</v>
       </c>
@@ -33386,7 +33386,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="292" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>1103</v>
       </c>
@@ -33766,7 +33766,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="296" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>1103</v>
       </c>
@@ -34051,7 +34051,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="299" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>1125</v>
       </c>
@@ -35191,7 +35191,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="311" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>1143</v>
       </c>
@@ -35476,7 +35476,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="314" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>1143</v>
       </c>
@@ -35571,7 +35571,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="315" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>1176</v>
       </c>
@@ -35761,7 +35761,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="317" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>1182</v>
       </c>
@@ -38231,7 +38231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="343" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>1264</v>
       </c>
@@ -38611,7 +38611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="347" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>1286</v>
       </c>
@@ -38896,7 +38896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="350" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:31" ht="360" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>1301</v>
       </c>
@@ -39371,7 +39371,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="355" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>1307</v>
       </c>
@@ -39561,7 +39561,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="357" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>1322</v>
       </c>
@@ -39846,7 +39846,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="360" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:31" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>1336</v>
       </c>
@@ -40036,7 +40036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="362" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>1350</v>
       </c>
@@ -40131,7 +40131,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="363" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:31" ht="288" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>1350</v>
       </c>
@@ -40511,7 +40511,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="367" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>1373</v>
       </c>
@@ -40606,7 +40606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="368" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:31" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>1373</v>
       </c>
@@ -40701,7 +40701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="369" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>1380</v>
       </c>
@@ -41081,7 +41081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="373" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:31" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>1399</v>
       </c>
@@ -41651,7 +41651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="379" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>1432</v>
       </c>
@@ -41841,7 +41841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="381" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:31" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>1447</v>
       </c>
@@ -41936,7 +41936,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="382" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>1455</v>
       </c>
@@ -42041,8 +42041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8A6D3B-FA95-4E67-9F6B-F1AE98A40FB8}">
   <dimension ref="A1:Z127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>